<commit_message>
Agile Updated (login page assignation)
</commit_message>
<xml_diff>
--- a/Management/Agile.xlsx
+++ b/Management/Agile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358A48E4-A825-4912-99E3-EC0A59462DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDAB43A-74C6-4311-81D3-BB1D080F922C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -789,6 +789,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,15 +825,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1738,8 +1738,8 @@
   </sheetPr>
   <dimension ref="A1:BL38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B22" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1805,39 +1805,39 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="61" t="s">
+      <c r="I2" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="N2" s="62" t="s">
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="N2" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="63" t="s">
+      <c r="S2" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="54" t="s">
+      <c r="X2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
+      <c r="Y2" s="57"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="57"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="55" t="s">
+      <c r="AC2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -1847,24 +1847,24 @@
         <v>40</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="59">
+      <c r="E3" s="60"/>
+      <c r="F3" s="62">
         <v>44099</v>
       </c>
-      <c r="G3" s="60"/>
+      <c r="G3" s="63"/>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="57"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -1953,13 +1953,13 @@
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>44099</v>
@@ -2572,7 +2572,7 @@
       <c r="A9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="55" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="34"/>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="54" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="34"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="13" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="54" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="34"/>
@@ -3346,7 +3346,7 @@
     </row>
     <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="55" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="34"/>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="66"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
       <c r="E17" s="31"/>
@@ -4528,7 +4528,7 @@
     </row>
     <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="54" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="34"/>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="34" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E24" s="31"/>
       <c r="F24" s="32">

</xml_diff>